<commit_message>
Setting cloud role name
</commit_message>
<xml_diff>
--- a/UnderstandingLogging.xlsx
+++ b/UnderstandingLogging.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LearningApplicationInsights\learning-app-insights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F9C3984-7EC2-4A5B-99B6-1FE0FACDF486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C2CAE9-2777-407B-9805-F64DC5DD9535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
   <si>
     <t>App Service code less instrumentation</t>
   </si>
@@ -106,6 +107,102 @@
   </si>
   <si>
     <t>Both</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Yes
+Custom properties are logged in CustomDimensions</t>
+  </si>
+  <si>
+    <t>Yes (When logged with TrackDependencies)
+Not out of the box</t>
+  </si>
+  <si>
+    <t>Yes
+When logged its available
+Custom Properties are not coming
+Need to research for correlation
+It' looks possible but needs to be explored</t>
+  </si>
+  <si>
+    <t>Serilog Integration with Telemetry Client</t>
+  </si>
+  <si>
+    <t>Traces</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>Correlatable Fields</t>
+  </si>
+  <si>
+    <t>Custom Properties</t>
+  </si>
+  <si>
+    <t>AppId
+cloud_RoleInstance
+customDimensions.AzureFunctions_invocationId
+is present but doesn't look correlatable</t>
+  </si>
+  <si>
+    <t>There is no detail abou the resource that generated this trace item
+Must be manually configured</t>
+  </si>
+  <si>
+    <t>AppId
+Cloud_roleInstance are there correlatable with which application generated
+Nothing to corelate with the actual request</t>
+  </si>
+  <si>
+    <t>Sampling</t>
+  </si>
+  <si>
+    <t>Dependencies are getting sampled?</t>
+  </si>
+  <si>
+    <t>Manually tracked for HTTP</t>
+  </si>
+  <si>
+    <t>Dependencies HTTP</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Event</t>
+  </si>
+  <si>
+    <t>Metric</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
+  </si>
+  <si>
+    <t>Integration type</t>
+  </si>
+  <si>
+    <t>Serilog-TelemetryClient</t>
+  </si>
+  <si>
+    <t>AppService</t>
+  </si>
+  <si>
+    <t>Request(Http)</t>
   </si>
 </sst>
 </file>
@@ -149,9 +246,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,183 +532,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="B1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="44.46484375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.9296875" customWidth="1"/>
-    <col min="5" max="5" width="43.1328125" customWidth="1"/>
+    <col min="2" max="2" width="44.46484375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.59765625" customWidth="1"/>
+    <col min="5" max="5" width="18.9296875" customWidth="1"/>
+    <col min="6" max="6" width="43.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="B1" t="s">
+    <row r="1" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+      <c r="D4" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
+    <row r="11" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B11" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
+    <row r="13" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B13" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
+    <row r="14" spans="2:6" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B14" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
+      <c r="D14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
+    <row r="16" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B16" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B21" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B24" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A25" t="s">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B25" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A26" t="s">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A28" t="s">
+    <row r="28" spans="2:4" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B28" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A29" t="s">
+      <c r="D28" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B29" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A30" t="s">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A31" t="s">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A32" t="s">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B32" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A35" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F0A6E6-3ED1-4D78-8A55-5E16B5C2D919}">
+  <dimension ref="A1:K12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33" customWidth="1"/>
+    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53.73046875" customWidth="1"/>
+    <col min="6" max="6" width="54.796875" customWidth="1"/>
+    <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.06640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Made couple of changes
</commit_message>
<xml_diff>
--- a/UnderstandingLogging.xlsx
+++ b/UnderstandingLogging.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LearningApplicationInsights\learning-app-insights\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C2CAE9-2777-407B-9805-F64DC5DD9535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781AB08F-5A69-483B-9F0C-661BE76125DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
   <si>
     <t>App Service code less instrumentation</t>
   </si>
@@ -133,9 +133,6 @@
 It' looks possible but needs to be explored</t>
   </si>
   <si>
-    <t>Serilog Integration with Telemetry Client</t>
-  </si>
-  <si>
     <t>Traces</t>
   </si>
   <si>
@@ -154,30 +151,12 @@
     <t>Custom Properties</t>
   </si>
   <si>
-    <t>AppId
-cloud_RoleInstance
-customDimensions.AzureFunctions_invocationId
-is present but doesn't look correlatable</t>
-  </si>
-  <si>
-    <t>There is no detail abou the resource that generated this trace item
-Must be manually configured</t>
-  </si>
-  <si>
-    <t>AppId
-Cloud_roleInstance are there correlatable with which application generated
-Nothing to corelate with the actual request</t>
-  </si>
-  <si>
     <t>Sampling</t>
   </si>
   <si>
     <t>Dependencies are getting sampled?</t>
   </si>
   <si>
-    <t>Manually tracked for HTTP</t>
-  </si>
-  <si>
     <t>Dependencies HTTP</t>
   </si>
   <si>
@@ -203,6 +182,53 @@
   </si>
   <si>
     <t>Request(Http)</t>
+  </si>
+  <si>
+    <t>Manually tracked for HTTP
+The cloud role name has to be set</t>
+  </si>
+  <si>
+    <t>Cloud application identifier</t>
+  </si>
+  <si>
+    <t>Cloud Instance Identifier</t>
+  </si>
+  <si>
+    <t>Executing identifier</t>
+  </si>
+  <si>
+    <t>Distributed transaction identifier</t>
+  </si>
+  <si>
+    <t>customDimensions.InvocationId</t>
+  </si>
+  <si>
+    <t>customDimensions.HostInstanceId</t>
+  </si>
+  <si>
+    <t>cloud_RoleName</t>
+  </si>
+  <si>
+    <t>UserCorrelation</t>
+  </si>
+  <si>
+    <t>Relook needed (Using deprecated API)</t>
+  </si>
+  <si>
+    <t>appID?</t>
+  </si>
+  <si>
+    <t>FileCorrelation/Module Correlation</t>
+  </si>
+  <si>
+    <t>customDimensions.Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No (As all the logs have come to the console)
+Need to check about </t>
+  </si>
+  <si>
+    <t>Per log property for traces</t>
   </si>
 </sst>
 </file>
@@ -732,27 +758,96 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03F0A6E6-3ED1-4D78-8A55-5E16B5C2D919}">
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="33" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.3984375" customWidth="1"/>
+    <col min="3" max="3" width="36.46484375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="53.73046875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.73046875" customWidth="1"/>
-    <col min="6" max="6" width="54.796875" customWidth="1"/>
+    <col min="6" max="6" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.9296875" customWidth="1"/>
+    <col min="8" max="8" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.06640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" t="s">
         <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.45">
@@ -760,156 +855,208 @@
         <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="F3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="H3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
       </c>
-      <c r="E4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="57" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G6" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="J6" t="s">
+        <v>29</v>
+      </c>
+      <c r="K6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
+        <v>55</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J7" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" t="s">
-        <v>47</v>
+        <v>42</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="J8" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" t="s">
-        <v>47</v>
-      </c>
-      <c r="K9" s="2"/>
+        <v>37</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>54</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
+        <v>39</v>
+      </c>
+      <c r="D10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E11" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" t="s">
-        <v>29</v>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>